<commit_message>
- Updated UI (now using bootstrap 3) - Multiple program slots - Pain rating/recording functionality - Audio prompts for participants - Better documentation and code comments - More options from command line (--no-box, --debug, --port) - Auto select all of console text for easy copy-paste - Better log management (should be windows compatible)
</commit_message>
<xml_diff>
--- a/docs/pressures.xlsx
+++ b/docs/pressures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="2700" windowWidth="19080" windowHeight="17080" tabRatio="500"/>
+    <workbookView xWindow="760" yWindow="0" windowWidth="19080" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,8 +101,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -144,7 +152,7 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -160,6 +168,10 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -175,6 +187,10 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,7 +523,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>